<commit_message>
Cambios Spline Sección Interpolación (Orden de los puntos)
</commit_message>
<xml_diff>
--- a/app/tables/tabla_newtonint.xlsx
+++ b/app/tables/tabla_newtonint.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>-3</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -449,16 +449,66 @@
           <t>0</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="C2" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
         <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-4</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>